<commit_message>
Added parsing transactions with support both account and origin currency amount. Completed relevant fixes and enhancements for Beancount report.
</commit_message>
<xml_diff>
--- a/testdata/ineco/valid_card.xlsx
+++ b/testdata/ineco/valid_card.xlsx
@@ -427,7 +427,7 @@
     <t xml:space="preserve">05/06/2024</t>
   </si>
   <si>
-    <t xml:space="preserve">-100.10</t>
+    <t xml:space="preserve">-350.00</t>
   </si>
   <si>
     <t xml:space="preserve">06/06/2024</t>
@@ -528,7 +528,7 @@
     <numFmt numFmtId="173" formatCode="@"/>
     <numFmt numFmtId="174" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -754,6 +754,12 @@
       <name val="GHEA Grapalat"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
+      <name val="GHEA Grapalat"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="8.5"/>
@@ -959,7 +965,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1192,7 +1198,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="32" fillId="2" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="32" fillId="2" borderId="2" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="33" fillId="2" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1200,7 +1210,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="2" borderId="2" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="2" borderId="2" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1220,7 +1230,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="2" borderId="2" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="2" borderId="2" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1228,11 +1238,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="2" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="2" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="2" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="2" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1350,9 +1360,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>27720</xdr:colOff>
+      <xdr:colOff>27360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1366,7 +1376,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1438200" cy="375120"/>
+          <a:ext cx="1437840" cy="374760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1389,7 +1399,7 @@
   <dimension ref="A2:AF1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB4" activeCellId="0" sqref="AB4"/>
+      <selection pane="topLeft" activeCell="R29" activeCellId="0" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2153,7 +2163,7 @@
         <v>51</v>
       </c>
       <c r="B21" s="51" t="n">
-        <v>1980</v>
+        <v>350</v>
       </c>
       <c r="C21" s="51"/>
       <c r="D21" s="52" t="s">
@@ -2281,10 +2291,10 @@
       <c r="A24" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="51" t="n">
-        <v>12000</v>
-      </c>
-      <c r="C24" s="51"/>
+      <c r="B24" s="58" t="n">
+        <v>999999999.99</v>
+      </c>
+      <c r="C24" s="58"/>
       <c r="D24" s="52" t="s">
         <v>11</v>
       </c>
@@ -2360,7 +2370,7 @@
       <c r="AE25" s="57"/>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="58"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -2385,321 +2395,321 @@
       <c r="J27" s="47"/>
       <c r="K27" s="47"/>
       <c r="L27" s="47"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="59"/>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="59"/>
-      <c r="W27" s="59"/>
-      <c r="X27" s="59"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="60"/>
+      <c r="T27" s="60"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="60"/>
+      <c r="W27" s="60"/>
+      <c r="X27" s="60"/>
       <c r="Y27" s="21"/>
       <c r="Z27" s="21"/>
       <c r="AA27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="61" t="s">
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61" t="s">
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="L28" s="61"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="59"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="59"/>
-      <c r="W28" s="59"/>
-      <c r="X28" s="59"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="60"/>
+      <c r="T28" s="60"/>
+      <c r="U28" s="60"/>
+      <c r="V28" s="60"/>
+      <c r="W28" s="60"/>
+      <c r="X28" s="60"/>
       <c r="Y28" s="21"/>
       <c r="Z28" s="21"/>
       <c r="AA28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="62" t="s">
+      <c r="A29" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="63" t="s">
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="L29" s="63"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-      <c r="R29" s="59"/>
-      <c r="S29" s="59"/>
-      <c r="T29" s="64"/>
-      <c r="U29" s="64"/>
-      <c r="V29" s="64"/>
-      <c r="W29" s="64"/>
-      <c r="X29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="60"/>
+      <c r="T29" s="65"/>
+      <c r="U29" s="65"/>
+      <c r="V29" s="65"/>
+      <c r="W29" s="65"/>
+      <c r="X29" s="65"/>
       <c r="Y29" s="21"/>
       <c r="Z29" s="21"/>
       <c r="AA29" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="63" t="n">
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="64" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="63"/>
-      <c r="J30" s="63"/>
-      <c r="K30" s="63" t="s">
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="L30" s="63"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="59"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="59"/>
-      <c r="R30" s="59"/>
-      <c r="S30" s="59"/>
-      <c r="T30" s="59"/>
-      <c r="U30" s="59"/>
-      <c r="V30" s="59"/>
-      <c r="W30" s="59"/>
-      <c r="X30" s="59"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="60"/>
+      <c r="T30" s="60"/>
+      <c r="U30" s="60"/>
+      <c r="V30" s="60"/>
+      <c r="W30" s="60"/>
+      <c r="X30" s="60"/>
       <c r="Y30" s="21"/>
       <c r="Z30" s="21"/>
       <c r="AA30" s="21"/>
     </row>
     <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="63" t="n">
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="64" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63" t="s">
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="L31" s="63"/>
+      <c r="L31" s="64"/>
       <c r="AF31" s="21"/>
     </row>
     <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="62" t="s">
+      <c r="A32" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="62"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="63" t="s">
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="63"/>
+      <c r="L32" s="64"/>
       <c r="AF32" s="21"/>
     </row>
     <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="62" t="s">
+      <c r="A33" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="63" t="s">
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="L33" s="63"/>
+      <c r="L33" s="64"/>
       <c r="AF33" s="21"/>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="67"/>
-      <c r="O35" s="67"/>
-      <c r="P35" s="67"/>
-      <c r="Q35" s="67"/>
-      <c r="R35" s="67"/>
-      <c r="S35" s="67"/>
-      <c r="T35" s="67"/>
-      <c r="U35" s="67"/>
-      <c r="V35" s="67"/>
-      <c r="W35" s="67"/>
-      <c r="X35" s="67"/>
-      <c r="Y35" s="67"/>
-      <c r="Z35" s="67"/>
-      <c r="AA35" s="67"/>
-      <c r="AB35" s="67"/>
-      <c r="AC35" s="67"/>
-      <c r="AD35" s="67"/>
-      <c r="AE35" s="67"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
+      <c r="Q35" s="68"/>
+      <c r="R35" s="68"/>
+      <c r="S35" s="68"/>
+      <c r="T35" s="68"/>
+      <c r="U35" s="68"/>
+      <c r="V35" s="68"/>
+      <c r="W35" s="68"/>
+      <c r="X35" s="68"/>
+      <c r="Y35" s="68"/>
+      <c r="Z35" s="68"/>
+      <c r="AA35" s="68"/>
+      <c r="AB35" s="68"/>
+      <c r="AC35" s="68"/>
+      <c r="AD35" s="68"/>
+      <c r="AE35" s="68"/>
     </row>
     <row r="37" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="68" t="s">
+      <c r="A37" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="68"/>
-      <c r="P37" s="68"/>
-      <c r="Q37" s="68"/>
-      <c r="R37" s="68"/>
-      <c r="S37" s="68"/>
-      <c r="T37" s="68"/>
-      <c r="U37" s="68"/>
-      <c r="V37" s="68"/>
-      <c r="W37" s="68"/>
-      <c r="X37" s="68"/>
-      <c r="Y37" s="68"/>
-      <c r="Z37" s="68"/>
-      <c r="AA37" s="68"/>
-      <c r="AB37" s="68"/>
-      <c r="AC37" s="68"/>
-      <c r="AD37" s="68"/>
-      <c r="AE37" s="68"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="69"/>
+      <c r="Q37" s="69"/>
+      <c r="R37" s="69"/>
+      <c r="S37" s="69"/>
+      <c r="T37" s="69"/>
+      <c r="U37" s="69"/>
+      <c r="V37" s="69"/>
+      <c r="W37" s="69"/>
+      <c r="X37" s="69"/>
+      <c r="Y37" s="69"/>
+      <c r="Z37" s="69"/>
+      <c r="AA37" s="69"/>
+      <c r="AB37" s="69"/>
+      <c r="AC37" s="69"/>
+      <c r="AD37" s="69"/>
+      <c r="AE37" s="69"/>
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="69"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="69"/>
-      <c r="K38" s="69"/>
-      <c r="L38" s="69"/>
-      <c r="M38" s="69"/>
-      <c r="N38" s="69"/>
-      <c r="O38" s="69"/>
-      <c r="P38" s="69"/>
-      <c r="Q38" s="69"/>
-      <c r="R38" s="69"/>
-      <c r="S38" s="69"/>
-      <c r="T38" s="69"/>
-      <c r="U38" s="69"/>
-      <c r="V38" s="69"/>
-      <c r="W38" s="69"/>
-      <c r="X38" s="69"/>
-      <c r="Y38" s="69"/>
-      <c r="Z38" s="69"/>
-      <c r="AA38" s="69"/>
-      <c r="AB38" s="69"/>
-      <c r="AC38" s="69"/>
-      <c r="AD38" s="69"/>
-      <c r="AE38" s="69"/>
+      <c r="A38" s="70"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="70"/>
+      <c r="N38" s="70"/>
+      <c r="O38" s="70"/>
+      <c r="P38" s="70"/>
+      <c r="Q38" s="70"/>
+      <c r="R38" s="70"/>
+      <c r="S38" s="70"/>
+      <c r="T38" s="70"/>
+      <c r="U38" s="70"/>
+      <c r="V38" s="70"/>
+      <c r="W38" s="70"/>
+      <c r="X38" s="70"/>
+      <c r="Y38" s="70"/>
+      <c r="Z38" s="70"/>
+      <c r="AA38" s="70"/>
+      <c r="AB38" s="70"/>
+      <c r="AC38" s="70"/>
+      <c r="AD38" s="70"/>
+      <c r="AE38" s="70"/>
     </row>
     <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="70" t="s">
+      <c r="A39" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
-      <c r="H39" s="70"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="70"/>
-      <c r="K39" s="70"/>
-      <c r="L39" s="70"/>
-      <c r="M39" s="70"/>
-      <c r="N39" s="70"/>
-      <c r="O39" s="70"/>
-      <c r="P39" s="70"/>
-      <c r="Q39" s="70"/>
-      <c r="R39" s="70"/>
-      <c r="S39" s="70"/>
-      <c r="T39" s="70"/>
-      <c r="U39" s="70"/>
-      <c r="V39" s="70"/>
-      <c r="W39" s="70"/>
-      <c r="X39" s="70"/>
-      <c r="Y39" s="70"/>
-      <c r="Z39" s="70"/>
-      <c r="AA39" s="70"/>
-      <c r="AB39" s="70"/>
-      <c r="AC39" s="70"/>
-      <c r="AD39" s="70"/>
-      <c r="AE39" s="70"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
+      <c r="K39" s="71"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="71"/>
+      <c r="N39" s="71"/>
+      <c r="O39" s="71"/>
+      <c r="P39" s="71"/>
+      <c r="Q39" s="71"/>
+      <c r="R39" s="71"/>
+      <c r="S39" s="71"/>
+      <c r="T39" s="71"/>
+      <c r="U39" s="71"/>
+      <c r="V39" s="71"/>
+      <c r="W39" s="71"/>
+      <c r="X39" s="71"/>
+      <c r="Y39" s="71"/>
+      <c r="Z39" s="71"/>
+      <c r="AA39" s="71"/>
+      <c r="AB39" s="71"/>
+      <c r="AC39" s="71"/>
+      <c r="AD39" s="71"/>
+      <c r="AE39" s="71"/>
     </row>
     <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="21"/>
@@ -2892,7 +2902,7 @@
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C25 O23:O25 A21:C22 A23:B25 F21:O22 F23:N25 D22:E22">
+  <conditionalFormatting sqref="C23:C25 A21:C22 A23:B25 F21:O25 D22:E22">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>""</formula>
     </cfRule>

</xml_diff>